<commit_message>
Added functionality to generate correlations
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>T</t>
   </si>
@@ -61,10 +61,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,16 +103,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -140,6 +204,204 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Correlations!$B$13:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>T (Temp)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P (Pressure)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>U (Humidity)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ff (Wind Speed)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Td (Dew point Temp)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Correlations!$C$13:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.063133</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.014294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.042903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.010847</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.049012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2093133880"/>
+        <c:axId val="-2093204008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2093133880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093204008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2093204008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:tint val="75000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093133880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H10"/>
+  <dimension ref="B3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,16 +855,66 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>-6.3132999999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>-1.4293999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>4.2902999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>1.0847000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>-4.9012E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:H10">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C18">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>